<commit_message>
update dataset: compra agora
</commit_message>
<xml_diff>
--- a/Compra agora profile.xlsx
+++ b/Compra agora profile.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rogério-artigiani-cspo-psm-b882a911</t>
+          <t>https://www.linkedin.com/in/rogério-artigiani-cspo-psm-b882a911</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cristiane-antunes</t>
+          <t>https://www.linkedin.com/in/cristiane-antunes</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>welder-soares-leitão-83a14710a</t>
+          <t>https://www.linkedin.com/in/welder-soares-leitão-83a14710a</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>geovanaferreira</t>
+          <t>https://www.linkedin.com/in/geovanaferreira</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jcampos3</t>
+          <t>https://www.linkedin.com/in/jcampos3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>aline-s-bb5938117</t>
+          <t>https://www.linkedin.com/in/aline-s-bb5938117</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>fernanda-liveri-19a59522</t>
+          <t>https://www.linkedin.com/in/fernanda-liveri-19a59522</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>anapbatista</t>
+          <t>https://www.linkedin.com/in/anapbatista</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gabrielssian</t>
+          <t>https://www.linkedin.com/in/gabrielssian</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>kelly-cristina-deniz-2598a722</t>
+          <t>https://www.linkedin.com/in/kelly-cristina-deniz-2598a722</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gustavosilveira12</t>
+          <t>https://www.linkedin.com/in/gustavosilveira12</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jéssica-cristine-alexandrino-marcondes-68232751</t>
+          <t>https://www.linkedin.com/in/jéssica-cristine-alexandrino-marcondes-68232751</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>renan-t-ramos-1602b669</t>
+          <t>https://www.linkedin.com/in/renan-t-ramos-1602b669</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>brunoac19</t>
+          <t>https://www.linkedin.com/in/brunoac19</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>felipe-artur-rodrigues-batista-de-oliveira-366b3234</t>
+          <t>https://www.linkedin.com/in/felipe-artur-rodrigues-batista-de-oliveira-366b3234</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>fabio-senatore</t>
+          <t>https://www.linkedin.com/in/fabio-senatore</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>juliana-fava-canabrava-b44893168</t>
+          <t>https://www.linkedin.com/in/juliana-fava-canabrava-b44893168</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>isaac-de-freitas-lima-2a3567196</t>
+          <t>https://www.linkedin.com/in/isaac-de-freitas-lima-2a3567196</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>giangagliardo</t>
+          <t>https://www.linkedin.com/in/giangagliardo</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>bruno-medeiros-50396a48</t>
+          <t>https://www.linkedin.com/in/bruno-medeiros-50396a48</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>markosmadeira</t>
+          <t>https://www.linkedin.com/in/markosmadeira</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>olívia-longarço-6a747b</t>
+          <t>https://www.linkedin.com/in/olívia-longarço-6a747b</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>guilherme-vieira-15217565</t>
+          <t>https://www.linkedin.com/in/guilherme-vieira-15217565</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>adriel-dantas-44162873</t>
+          <t>https://www.linkedin.com/in/adriel-dantas-44162873</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>viniciusdiaspeixoto</t>
+          <t>https://www.linkedin.com/in/viniciusdiaspeixoto</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>alexsandro-souza-xavier-b5605959</t>
+          <t>https://www.linkedin.com/in/alexsandro-souza-xavier-b5605959</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>thaisehagge</t>
+          <t>https://www.linkedin.com/in/thaisehagge</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>roberta-rodrigues-muoio-b53a4733</t>
+          <t>https://www.linkedin.com/in/roberta-rodrigues-muoio-b53a4733</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>wesleinunes</t>
+          <t>https://www.linkedin.com/in/wesleinunes</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>sérgio-sobrosa-batista-30a9b61a6</t>
+          <t>https://www.linkedin.com/in/sérgio-sobrosa-batista-30a9b61a6</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>juliana-carsoni-19376553</t>
+          <t>https://www.linkedin.com/in/juliana-carsoni-19376553</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3575,7 +3575,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>miltonbarros</t>
+          <t>https://www.linkedin.com/in/miltonbarros</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tiago-vian-47a6ab11a</t>
+          <t>https://www.linkedin.com/in/tiago-vian-47a6ab11a</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>gustavo-p-barros-06249a67</t>
+          <t>https://www.linkedin.com/in/gustavo-p-barros-06249a67</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>camilasobral</t>
+          <t>https://www.linkedin.com/in/camilasobral</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -4057,7 +4057,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>álvaro-souza-a07a21a4</t>
+          <t>https://www.linkedin.com/in/álvaro-souza-a07a21a4</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>thiago-mendes-do-nascimento</t>
+          <t>https://www.linkedin.com/in/thiago-mendes-do-nascimento</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>carolinapirmez</t>
+          <t>https://www.linkedin.com/in/carolinapirmez</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>meire-hellen-galinari-lopes-bb2a18a0</t>
+          <t>https://www.linkedin.com/in/meire-hellen-galinari-lopes-bb2a18a0</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>aline-miura-b8187296</t>
+          <t>https://www.linkedin.com/in/aline-miura-b8187296</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -4624,7 +4624,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>daysy-andrade-silva-756876b2</t>
+          <t>https://www.linkedin.com/in/daysy-andrade-silva-756876b2</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>andressa-alves-3703a453</t>
+          <t>https://www.linkedin.com/in/andressa-alves-3703a453</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -4816,7 +4816,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>thais-vergueiro-6536b926</t>
+          <t>https://www.linkedin.com/in/thais-vergueiro-6536b926</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>cristina-baik-8b8b7749</t>
+          <t>https://www.linkedin.com/in/cristina-baik-8b8b7749</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5007,7 +5007,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>patriciagoia</t>
+          <t>https://www.linkedin.com/in/patriciagoia</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>rayssa-albuquerque-62581539</t>
+          <t>https://www.linkedin.com/in/rayssa-albuquerque-62581539</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>aline-portella-17755764</t>
+          <t>https://www.linkedin.com/in/aline-portella-17755764</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>silvana-fernandes-585b74</t>
+          <t>https://www.linkedin.com/in/silvana-fernandes-585b74</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -5440,7 +5440,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>beatrizcapistrano</t>
+          <t>https://www.linkedin.com/in/beatrizcapistrano</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ronaldoschulze</t>
+          <t>https://www.linkedin.com/in/ronaldoschulze</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">

</xml_diff>